<commit_message>
cleanup log files, finalize graphs, report mostly finished.
</commit_message>
<xml_diff>
--- a/results/bitonicsort.xlsx
+++ b/results/bitonicsort.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ValkCoen\Documents\school\parallel_prog\CSCI4320-FinalProject\results\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{29D43737-7DC2-43C1-9C32-5E0F27FEF2BA}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8E70CD52-8E37-44EC-8F41-706AA1C2C9C8}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{D18E6C05-0C84-4820-B53C-5AA539CD7F37}"/>
   </bookViews>
@@ -28,6 +28,14 @@
     </ext>
   </extLst>
 </workbook>
+</file>
+
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1" uniqueCount="1">
+  <si>
+    <t>Quicksort</t>
+  </si>
+</sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
@@ -95,378 +103,6 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
-      <c:overlay val="0"/>
-      <c:spPr>
-        <a:noFill/>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-        <a:effectLst/>
-      </c:spPr>
-      <c:txPr>
-        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr>
-            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="65000"/>
-                  <a:lumOff val="35000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:defRPr>
-          </a:pPr>
-          <a:endParaRPr lang="en-US"/>
-        </a:p>
-      </c:txPr>
-    </c:title>
-    <c:autoTitleDeleted val="0"/>
-    <c:plotArea>
-      <c:layout/>
-      <c:scatterChart>
-        <c:scatterStyle val="lineMarker"/>
-        <c:varyColors val="0"/>
-        <c:ser>
-          <c:idx val="0"/>
-          <c:order val="0"/>
-          <c:tx>
-            <c:strRef>
-              <c:f>Sheet1!$B$1</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>1048576</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:tx>
-          <c:spPr>
-            <a:ln w="19050" cap="rnd">
-              <a:solidFill>
-                <a:schemeClr val="accent1"/>
-              </a:solidFill>
-              <a:round/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:marker>
-            <c:symbol val="circle"/>
-            <c:size val="5"/>
-            <c:spPr>
-              <a:solidFill>
-                <a:schemeClr val="accent1"/>
-              </a:solidFill>
-              <a:ln w="9525">
-                <a:solidFill>
-                  <a:schemeClr val="accent1"/>
-                </a:solidFill>
-              </a:ln>
-              <a:effectLst/>
-            </c:spPr>
-          </c:marker>
-          <c:xVal>
-            <c:numRef>
-              <c:f>Sheet1!$A$2:$A$13</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="12"/>
-                <c:pt idx="0">
-                  <c:v>2</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>4</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>8</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>16</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>32</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>64</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>128</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>256</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>512</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>1024</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>2048</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>4096</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:xVal>
-          <c:yVal>
-            <c:numRef>
-              <c:f>Sheet1!$B$2:$B$13</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="12"/>
-                <c:pt idx="0">
-                  <c:v>5.6481950000000003</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>2.8351000000000002</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>1.4258729999999999</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>0.71909800000000001</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>0.36506699999999997</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>0.18707499999999999</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>9.7921999999999995E-2</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>5.2689E-2</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>3.048E-2</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>1.9050000000000001E-2</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>1.3672E-2</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>1.2108000000000001E-2</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:yVal>
-          <c:smooth val="0"/>
-          <c:extLst>
-            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000000-8055-49C6-8C47-F0D160486812}"/>
-            </c:ext>
-          </c:extLst>
-        </c:ser>
-        <c:dLbls>
-          <c:showLegendKey val="0"/>
-          <c:showVal val="0"/>
-          <c:showCatName val="0"/>
-          <c:showSerName val="0"/>
-          <c:showPercent val="0"/>
-          <c:showBubbleSize val="0"/>
-        </c:dLbls>
-        <c:axId val="659520672"/>
-        <c:axId val="659335664"/>
-      </c:scatterChart>
-      <c:valAx>
-        <c:axId val="659520672"/>
-        <c:scaling>
-          <c:orientation val="minMax"/>
-        </c:scaling>
-        <c:delete val="0"/>
-        <c:axPos val="b"/>
-        <c:majorGridlines>
-          <c:spPr>
-            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="15000"/>
-                  <a:lumOff val="85000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:round/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-        </c:majorGridlines>
-        <c:numFmt formatCode="General" sourceLinked="1"/>
-        <c:majorTickMark val="none"/>
-        <c:minorTickMark val="none"/>
-        <c:tickLblPos val="nextTo"/>
-        <c:spPr>
-          <a:noFill/>
-          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-            <a:solidFill>
-              <a:schemeClr val="tx1">
-                <a:lumMod val="25000"/>
-                <a:lumOff val="75000"/>
-              </a:schemeClr>
-            </a:solidFill>
-            <a:round/>
-          </a:ln>
-          <a:effectLst/>
-        </c:spPr>
-        <c:txPr>
-          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                <a:solidFill>
-                  <a:schemeClr val="tx1">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
-                  </a:schemeClr>
-                </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
-                <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
-              </a:defRPr>
-            </a:pPr>
-            <a:endParaRPr lang="en-US"/>
-          </a:p>
-        </c:txPr>
-        <c:crossAx val="659335664"/>
-        <c:crosses val="autoZero"/>
-        <c:crossBetween val="midCat"/>
-      </c:valAx>
-      <c:valAx>
-        <c:axId val="659335664"/>
-        <c:scaling>
-          <c:orientation val="minMax"/>
-        </c:scaling>
-        <c:delete val="0"/>
-        <c:axPos val="l"/>
-        <c:majorGridlines>
-          <c:spPr>
-            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="15000"/>
-                  <a:lumOff val="85000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:round/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-        </c:majorGridlines>
-        <c:numFmt formatCode="General" sourceLinked="1"/>
-        <c:majorTickMark val="none"/>
-        <c:minorTickMark val="none"/>
-        <c:tickLblPos val="nextTo"/>
-        <c:spPr>
-          <a:noFill/>
-          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-            <a:solidFill>
-              <a:schemeClr val="tx1">
-                <a:lumMod val="25000"/>
-                <a:lumOff val="75000"/>
-              </a:schemeClr>
-            </a:solidFill>
-            <a:round/>
-          </a:ln>
-          <a:effectLst/>
-        </c:spPr>
-        <c:txPr>
-          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                <a:solidFill>
-                  <a:schemeClr val="tx1">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
-                  </a:schemeClr>
-                </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
-                <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
-              </a:defRPr>
-            </a:pPr>
-            <a:endParaRPr lang="en-US"/>
-          </a:p>
-        </c:txPr>
-        <c:crossAx val="659520672"/>
-        <c:crosses val="autoZero"/>
-        <c:crossBetween val="midCat"/>
-      </c:valAx>
-      <c:spPr>
-        <a:noFill/>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-        <a:effectLst/>
-      </c:spPr>
-    </c:plotArea>
-    <c:plotVisOnly val="1"/>
-    <c:dispBlanksAs val="gap"/>
-    <c:extLst>
-      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
-        <c16r3:dataDisplayOptions16>
-          <c16r3:dispNaAsBlank val="1"/>
-        </c16r3:dataDisplayOptions16>
-      </c:ext>
-    </c:extLst>
-    <c:showDLblsOverMax val="0"/>
-  </c:chart>
-  <c:spPr>
-    <a:solidFill>
-      <a:schemeClr val="bg1"/>
-    </a:solidFill>
-    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-      <a:solidFill>
-        <a:schemeClr val="tx1">
-          <a:lumMod val="15000"/>
-          <a:lumOff val="85000"/>
-        </a:schemeClr>
-      </a:solidFill>
-      <a:round/>
-    </a:ln>
-    <a:effectLst/>
-  </c:spPr>
-  <c:txPr>
-    <a:bodyPr/>
-    <a:lstStyle/>
-    <a:p>
-      <a:pPr>
-        <a:defRPr/>
-      </a:pPr>
-      <a:endParaRPr lang="en-US"/>
-    </a:p>
-  </c:txPr>
-  <c:printSettings>
-    <c:headerFooter/>
-    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
-    <c:pageSetup/>
-  </c:printSettings>
-</c:chartSpace>
-</file>
-
-<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
-  <c:date1904 val="0"/>
-  <c:lang val="en-US"/>
-  <c:roundedCorners val="0"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
-      <c14:style val="102"/>
-    </mc:Choice>
-    <mc:Fallback>
-      <c:style val="2"/>
-    </mc:Fallback>
-  </mc:AlternateContent>
-  <c:chart>
-    <c:title>
       <c:tx>
         <c:rich>
           <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
@@ -487,13 +123,8 @@
             </a:pPr>
             <a:r>
               <a:rPr lang="en-US"/>
-              <a:t>Scalability of Bitonic Sort - 33554432</a:t>
+              <a:t>Scalability of Bitonic Mergesort</a:t>
             </a:r>
-            <a:r>
-              <a:rPr lang="en-US" baseline="0"/>
-              <a:t> Elements</a:t>
-            </a:r>
-            <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:rich>
       </c:tx>
@@ -537,11 +168,11 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$G$1</c:f>
+              <c:f>Sheet1!$B$1</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>33554432</c:v>
+                  <c:v>1048576</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -617,45 +248,45 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet1!$G$2:$G$13</c:f>
+              <c:f>Sheet1!$B$2:$B$13</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="12"/>
                 <c:pt idx="0">
-                  <c:v>277.43898899999999</c:v>
+                  <c:v>5.6481950000000003</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>138.92964699999999</c:v>
+                  <c:v>2.8351000000000002</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>69.700667999999993</c:v>
+                  <c:v>1.4258729999999999</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>35.032395999999999</c:v>
+                  <c:v>0.71909800000000001</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>17.666710999999999</c:v>
+                  <c:v>0.36506699999999997</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>8.9626140000000003</c:v>
+                  <c:v>0.18707499999999999</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>4.6071679999999997</c:v>
+                  <c:v>9.7921999999999995E-2</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>2.4073449999999998</c:v>
+                  <c:v>5.2689E-2</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>1.3045929999999999</c:v>
+                  <c:v>3.048E-2</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>0.75179600000000002</c:v>
+                  <c:v>1.9050000000000001E-2</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>0.47471099999999999</c:v>
+                  <c:v>1.3672E-2</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>0.36280200000000001</c:v>
+                  <c:v>1.2108000000000001E-2</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -663,7 +294,682 @@
           <c:smooth val="1"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000000-4D42-43BA-B4FD-39E1D69D6175}"/>
+              <c16:uniqueId val="{00000000-79E5-43C1-9467-A988C59DF859}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$C$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>2097152</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent2"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Sheet1!$A$2:$A$13</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="12"/>
+                <c:pt idx="0">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>32</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>64</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>128</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>256</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>512</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>1024</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>2048</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>4096</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Sheet1!$C$2:$C$13</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="12"/>
+                <c:pt idx="0">
+                  <c:v>12.40028</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>6.2184109999999997</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>3.1274980000000001</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1.5756399999999999</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.79829000000000006</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.40747</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.19584399999999999</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.105378</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>6.096E-2</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>3.8100000000000002E-2</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>2.7344E-2</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>2.4216000000000001E-2</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="1"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-79E5-43C1-9467-A988C59DF859}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$D$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>4194304</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent3"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent3"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent3"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Sheet1!$A$2:$A$13</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="12"/>
+                <c:pt idx="0">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>32</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>64</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>128</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>256</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>512</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>1024</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>2048</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>4096</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Sheet1!$D$2:$D$13</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="12"/>
+                <c:pt idx="0">
+                  <c:v>27.110648000000001</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>13.591623999999999</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>6.8249500000000003</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>3.4385370000000002</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1.7401549999999999</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.886019</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.39168799999999998</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.210756</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.12192</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>7.6200000000000004E-2</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>5.4688000000000001E-2</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>4.8432000000000003E-2</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="1"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000002-79E5-43C1-9467-A988C59DF859}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="3"/>
+          <c:order val="3"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$E$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>8388608</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent4"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent4"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent4"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Sheet1!$A$2:$A$13</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="12"/>
+                <c:pt idx="0">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>32</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>64</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>128</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>256</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>512</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>1024</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>2048</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>4096</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Sheet1!$E$2:$E$13</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="12"/>
+                <c:pt idx="0">
+                  <c:v>59.046550000000003</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>29.595894000000001</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>14.855981999999999</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>7.4725590000000004</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>3.780996</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1.921988</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.78337599999999996</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.421512</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.24384</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.15240000000000001</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0.109376</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>9.6864000000000006E-2</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="1"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000003-79E5-43C1-9467-A988C59DF859}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="4"/>
+          <c:order val="4"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$F$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>16777216</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent5"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent5"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent5"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Sheet1!$A$2:$A$13</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="12"/>
+                <c:pt idx="0">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>32</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>64</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>128</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>256</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>512</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>1024</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>2048</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>4096</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Sheet1!$F$2:$F$13</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="12"/>
+                <c:pt idx="0">
+                  <c:v>128.156094</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>64.226926000000006</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>32.23169</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>16.207636999999998</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>8.1780690000000007</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>4.1611669999999998</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>1.5667519999999999</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.843024</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.48768</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.30480000000000002</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0.218752</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>0.19372800000000001</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="1"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000004-79E5-43C1-9467-A988C59DF859}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="5"/>
+          <c:order val="5"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$G$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>33554432</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent6"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent6"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent6"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Sheet1!$A$2:$A$13</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="12"/>
+                <c:pt idx="0">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>32</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>64</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>128</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>256</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>512</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>1024</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>2048</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>4096</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Sheet1!$G$2:$G$13</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="12"/>
+                <c:pt idx="0">
+                  <c:v>277.43898899999999</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>138.92964699999999</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>69.700667999999993</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>35.032395999999999</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>17.666710999999999</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>8.9626140000000003</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>4.6071679999999997</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>2.4073449999999998</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>1.3045929999999999</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.75179600000000002</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0.47471099999999999</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>0.36280200000000001</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="1"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000005-79E5-43C1-9467-A988C59DF859}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -675,11 +981,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="665218864"/>
-        <c:axId val="659363536"/>
+        <c:axId val="526411312"/>
+        <c:axId val="524228960"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="665218864"/>
+        <c:axId val="526411312"/>
         <c:scaling>
           <c:logBase val="2"/>
           <c:orientation val="minMax"/>
@@ -797,13 +1103,14 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="659363536"/>
+        <c:crossAx val="524228960"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="659363536"/>
+        <c:axId val="524228960"/>
         <c:scaling>
+          <c:logBase val="10"/>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:delete val="0"/>
@@ -843,13 +1150,8 @@
                 </a:pPr>
                 <a:r>
                   <a:rPr lang="en-US"/>
-                  <a:t>Execution</a:t>
+                  <a:t>Execution Time (s)</a:t>
                 </a:r>
-                <a:r>
-                  <a:rPr lang="en-US" baseline="0"/>
-                  <a:t> Time (s)</a:t>
-                </a:r>
-                <a:endParaRPr lang="en-US"/>
               </a:p>
             </c:rich>
           </c:tx>
@@ -919,7 +1221,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="665218864"/>
+        <c:crossAx val="526411312"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -931,6 +1233,1670 @@
         <a:effectLst/>
       </c:spPr>
     </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>Execution</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US" baseline="0"/>
+              <a:t> Time Growth of Bitonic Mergesort</a:t>
+            </a:r>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="smoothMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$A$2</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>2</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Sheet1!$B$1:$G$1</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>1048576</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2097152</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>4194304</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>8388608</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>16777216</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>33554432</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Sheet1!$B$2:$G$2</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>5.6481950000000003</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>12.40028</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>27.110648000000001</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>59.046550000000003</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>128.156094</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>277.43898899999999</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="1"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-8075-4091-AFDA-145F8F916D50}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$A$3</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>4</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent2"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Sheet1!$B$1:$G$1</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>1048576</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2097152</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>4194304</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>8388608</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>16777216</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>33554432</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Sheet1!$B$3:$G$3</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>2.8351000000000002</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>6.2184109999999997</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>13.591623999999999</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>29.595894000000001</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>64.226926000000006</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>138.92964699999999</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="1"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-8075-4091-AFDA-145F8F916D50}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$A$4</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>8</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent3"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent3"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent3"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Sheet1!$B$1:$G$1</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>1048576</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2097152</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>4194304</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>8388608</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>16777216</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>33554432</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Sheet1!$B$4:$G$4</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>1.4258729999999999</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>3.1274980000000001</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>6.8249500000000003</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>14.855981999999999</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>32.23169</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>69.700667999999993</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="1"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000002-8075-4091-AFDA-145F8F916D50}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="3"/>
+          <c:order val="3"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$A$5</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>16</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent4"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent4"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent4"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Sheet1!$B$1:$G$1</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>1048576</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2097152</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>4194304</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>8388608</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>16777216</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>33554432</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Sheet1!$B$5:$G$5</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>0.71909800000000001</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1.5756399999999999</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>3.4385370000000002</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>7.4725590000000004</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>16.207636999999998</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>35.032395999999999</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="1"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000003-8075-4091-AFDA-145F8F916D50}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="4"/>
+          <c:order val="4"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$A$6</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>32</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent5"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent5"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent5"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Sheet1!$B$1:$G$1</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>1048576</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2097152</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>4194304</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>8388608</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>16777216</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>33554432</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Sheet1!$B$6:$G$6</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>0.36506699999999997</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.79829000000000006</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1.7401549999999999</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>3.780996</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>8.1780690000000007</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>17.666710999999999</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="1"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000004-8075-4091-AFDA-145F8F916D50}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="5"/>
+          <c:order val="5"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$A$7</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>64</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent6"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent6"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent6"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Sheet1!$B$1:$G$1</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>1048576</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2097152</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>4194304</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>8388608</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>16777216</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>33554432</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Sheet1!$B$7:$G$7</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>0.18707499999999999</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.40747</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.886019</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1.921988</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>4.1611669999999998</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>8.9626140000000003</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="1"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000005-8075-4091-AFDA-145F8F916D50}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="6"/>
+          <c:order val="6"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$A$8</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>128</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1">
+                  <a:lumMod val="60000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1">
+                  <a:lumMod val="60000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent1">
+                    <a:lumMod val="60000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Sheet1!$B$1:$G$1</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>1048576</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2097152</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>4194304</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>8388608</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>16777216</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>33554432</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Sheet1!$B$8:$G$8</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>9.7921999999999995E-2</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.19584399999999999</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.39168799999999998</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.78337599999999996</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1.5667519999999999</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>4.6071679999999997</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="1"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000006-8075-4091-AFDA-145F8F916D50}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="7"/>
+          <c:order val="7"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$A$9</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>256</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent2">
+                  <a:lumMod val="60000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent2">
+                  <a:lumMod val="60000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent2">
+                    <a:lumMod val="60000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Sheet1!$B$1:$G$1</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>1048576</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2097152</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>4194304</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>8388608</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>16777216</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>33554432</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Sheet1!$B$9:$G$9</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>5.2689E-2</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.105378</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.210756</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.421512</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.843024</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>2.4073449999999998</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="1"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000007-8075-4091-AFDA-145F8F916D50}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="8"/>
+          <c:order val="8"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$A$10</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>512</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent3">
+                  <a:lumMod val="60000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent3">
+                  <a:lumMod val="60000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent3">
+                    <a:lumMod val="60000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Sheet1!$B$1:$G$1</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>1048576</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2097152</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>4194304</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>8388608</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>16777216</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>33554432</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Sheet1!$B$10:$G$10</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>3.048E-2</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>6.096E-2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.12192</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.24384</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.48768</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1.3045929999999999</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="1"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000008-8075-4091-AFDA-145F8F916D50}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="9"/>
+          <c:order val="9"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$A$11</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>1024</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent4">
+                  <a:lumMod val="60000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent4">
+                  <a:lumMod val="60000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent4">
+                    <a:lumMod val="60000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Sheet1!$B$1:$G$1</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>1048576</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2097152</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>4194304</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>8388608</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>16777216</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>33554432</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Sheet1!$B$11:$G$11</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>1.9050000000000001E-2</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>3.8100000000000002E-2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>7.6200000000000004E-2</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.15240000000000001</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.30480000000000002</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.75179600000000002</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="1"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000009-8075-4091-AFDA-145F8F916D50}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="10"/>
+          <c:order val="10"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$A$12</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>2048</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent5">
+                  <a:lumMod val="60000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent5">
+                  <a:lumMod val="60000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent5">
+                    <a:lumMod val="60000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Sheet1!$B$1:$G$1</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>1048576</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2097152</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>4194304</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>8388608</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>16777216</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>33554432</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Sheet1!$B$12:$G$12</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>1.3672E-2</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2.7344E-2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>5.4688000000000001E-2</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.109376</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.218752</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.47471099999999999</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="1"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{0000000A-8075-4091-AFDA-145F8F916D50}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="11"/>
+          <c:order val="11"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$A$13</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>4096</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent6">
+                  <a:lumMod val="60000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent6">
+                  <a:lumMod val="60000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent6">
+                    <a:lumMod val="60000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Sheet1!$B$1:$G$1</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>1048576</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2097152</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>4194304</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>8388608</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>16777216</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>33554432</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Sheet1!$B$13:$G$13</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>1.2108000000000001E-2</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2.4216000000000001E-2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>4.8432000000000003E-2</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>9.6864000000000006E-2</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.19372800000000001</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.36280200000000001</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="1"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{0000000B-8075-4091-AFDA-145F8F916D50}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="561527040"/>
+        <c:axId val="563083360"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="561527040"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+          <c:min val="1048576"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Number of Elements</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="563083360"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="563083360"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Execution Time (s)</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="561527040"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="gap"/>
     <c:extLst>
@@ -1010,15 +2976,7 @@
             </a:pPr>
             <a:r>
               <a:rPr lang="en-US"/>
-              <a:t>Execution Time</a:t>
-            </a:r>
-            <a:r>
-              <a:rPr lang="en-US" baseline="0"/>
-              <a:t> of Bitoncisort - </a:t>
-            </a:r>
-            <a:r>
-              <a:rPr lang="en-US"/>
-              <a:t>64 ranks</a:t>
+              <a:t>Speedup of Bitonic Mergesort vs. Quicksort</a:t>
             </a:r>
           </a:p>
         </c:rich>
@@ -1056,18 +3014,18 @@
     <c:plotArea>
       <c:layout/>
       <c:scatterChart>
-        <c:scatterStyle val="lineMarker"/>
+        <c:scatterStyle val="smoothMarker"/>
         <c:varyColors val="0"/>
         <c:ser>
           <c:idx val="0"/>
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$A$7</c:f>
+              <c:f>Sheet1!$B$15</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>64</c:v>
+                  <c:v>1048576</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -1098,62 +3056,773 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>Sheet1!$B$1:$G$1</c:f>
+              <c:f>Sheet1!$A$16:$A$27</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="6"/>
-                <c:pt idx="0">
-                  <c:v>1048576</c:v>
+                <c:ptCount val="12"/>
+                <c:pt idx="0">
+                  <c:v>2</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>2097152</c:v>
+                  <c:v>4</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>4194304</c:v>
+                  <c:v>8</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>8388608</c:v>
+                  <c:v>16</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>16777216</c:v>
+                  <c:v>32</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>33554432</c:v>
+                  <c:v>64</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>128</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>256</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>512</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>1024</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>2048</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>4096</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet1!$B$7:$G$7</c:f>
+              <c:f>Sheet1!$B$16:$B$27</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="6"/>
-                <c:pt idx="0">
-                  <c:v>0.18707499999999999</c:v>
+                <c:ptCount val="12"/>
+                <c:pt idx="0">
+                  <c:v>0.28779123200000001</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.40747</c:v>
+                  <c:v>0.57334873500000005</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.886019</c:v>
+                  <c:v>1.140004054</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>1.921988</c:v>
+                  <c:v>2.2604721470000002</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>4.1611669999999998</c:v>
+                  <c:v>4.4526100690000003</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>8.9626140000000003</c:v>
+                  <c:v>8.6890338099999997</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>16.599957109999998</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>30.850860709999999</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>53.3300853</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>85.328136479999998</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>118.8927004</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>134.2501652</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:yVal>
-          <c:smooth val="0"/>
+          <c:smooth val="1"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000000-1E1C-4DA2-8720-EDB43258F15A}"/>
+              <c16:uniqueId val="{00000000-ECB4-4715-A409-DA8462011D65}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$C$15</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>2097152</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent2"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Sheet1!$A$16:$A$27</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="12"/>
+                <c:pt idx="0">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>32</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>64</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>128</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>256</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>512</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>1024</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>2048</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>4096</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Sheet1!$C$16:$C$27</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="12"/>
+                <c:pt idx="0">
+                  <c:v>0.28399987700000001</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.566330852</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1.1260368510000001</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>2.2350778099999999</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>4.4115271390000004</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>8.6427908799999997</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>17.982057149999999</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>33.419480350000001</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>57.770308399999998</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>92.432493440000002</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>128.79161790000001</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>145.4277337</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="1"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-ECB4-4715-A409-DA8462011D65}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$D$15</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>4194304</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent3"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent3"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent3"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Sheet1!$A$16:$A$27</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="12"/>
+                <c:pt idx="0">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>32</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>64</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>128</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>256</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>512</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>1024</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>2048</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>4096</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Sheet1!$D$16:$D$27</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="12"/>
+                <c:pt idx="0">
+                  <c:v>0.25604921000000003</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.510730727</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1.017100492</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>2.0187829879999999</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>3.9891044189999998</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>7.8346626879999999</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>17.722421929999999</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>32.936950789999997</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>56.936187660000002</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>91.097900260000003</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>126.93205089999999</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>143.32796500000001</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="1"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000002-ECB4-4715-A409-DA8462011D65}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="3"/>
+          <c:order val="3"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$E$15</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>8388608</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent4"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent4"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent4"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Sheet1!$A$16:$A$27</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="12"/>
+                <c:pt idx="0">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>32</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>64</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>128</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>256</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>512</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>1024</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>2048</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>4096</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Sheet1!$E$16:$E$27</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="12"/>
+                <c:pt idx="0">
+                  <c:v>0.24696225299999999</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.49271257000000002</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.98157556999999995</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1.951442471</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>3.8567269049999999</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>7.5870759860000003</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>18.614648649999999</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>34.59514557</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>59.802612369999999</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>95.684179790000002</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>133.32238330000001</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>150.5437417</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="1"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000003-ECB4-4715-A409-DA8462011D65}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="4"/>
+          <c:order val="4"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$F$15</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>16777216</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent5"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent5"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent5"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Sheet1!$A$16:$A$27</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="12"/>
+                <c:pt idx="0">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>32</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>64</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>128</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>256</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>512</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>1024</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>2048</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>4096</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Sheet1!$F$16:$F$27</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="12"/>
+                <c:pt idx="0">
+                  <c:v>0.231810561</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.46254644</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.92169960699999998</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1.8329591169999999</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>3.6326345500000001</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>7.1393279820000002</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>18.961479539999999</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>35.239727459999997</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>60.91686352</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>97.466981630000006</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>135.80646580000001</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>153.34869509999999</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="1"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000004-ECB4-4715-A409-DA8462011D65}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="5"/>
+          <c:order val="5"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$G$15</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>33554432</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent6"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent6"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent6"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Sheet1!$A$16:$A$27</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="12"/>
+                <c:pt idx="0">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>32</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>64</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>128</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>256</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>512</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>1024</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>2048</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>4096</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Sheet1!$G$16:$G$27</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="12"/>
+                <c:pt idx="0">
+                  <c:v>0.22991808799999999</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.45914060400000001</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.91517404099999999</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1.8208358339999999</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>3.6106461470000002</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>7.1171470729999999</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>13.84543433</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>26.497341259999999</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>48.895128210000003</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>84.847807119999999</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>134.37279100000001</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>175.82108700000001</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="1"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000005-ECB4-4715-A409-DA8462011D65}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -1165,11 +3834,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="659517872"/>
-        <c:axId val="667173168"/>
+        <c:axId val="356325840"/>
+        <c:axId val="479704096"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="659517872"/>
+        <c:axId val="356325840"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1210,7 +3879,11 @@
                 </a:pPr>
                 <a:r>
                   <a:rPr lang="en-US"/>
-                  <a:t>Number of Processors</a:t>
+                  <a:t>Number</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="en-US" baseline="0"/>
+                  <a:t> of Processes</a:t>
                 </a:r>
               </a:p>
             </c:rich>
@@ -1281,12 +3954,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="667173168"/>
+        <c:crossAx val="479704096"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="667173168"/>
+        <c:axId val="479704096"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1327,11 +4000,11 @@
                 </a:pPr>
                 <a:r>
                   <a:rPr lang="en-US"/>
-                  <a:t>Execution</a:t>
+                  <a:t>Times</a:t>
                 </a:r>
                 <a:r>
                   <a:rPr lang="en-US" baseline="0"/>
-                  <a:t> Time (s)</a:t>
+                  <a:t> Faster than Quicksort</a:t>
                 </a:r>
                 <a:endParaRPr lang="en-US"/>
               </a:p>
@@ -1403,7 +4076,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="659517872"/>
+        <c:crossAx val="356325840"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1415,6 +4088,37 @@
         <a:effectLst/>
       </c:spPr>
     </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="gap"/>
     <c:extLst>
@@ -3132,22 +5836,22 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>180975</xdr:colOff>
-      <xdr:row>16</xdr:row>
-      <xdr:rowOff>42862</xdr:rowOff>
+      <xdr:colOff>114300</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>33337</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>14</xdr:col>
-      <xdr:colOff>485775</xdr:colOff>
-      <xdr:row>30</xdr:row>
-      <xdr:rowOff>119062</xdr:rowOff>
+      <xdr:colOff>419100</xdr:colOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>109537</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="2" name="Chart 1">
+        <xdr:cNvPr id="5" name="Chart 4">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{3269A7DC-EB1D-47DD-8859-47D4546D249C}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{70798822-B3F2-44E9-9622-7006E73B3AED}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3167,23 +5871,23 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>7</xdr:col>
-      <xdr:colOff>161925</xdr:colOff>
-      <xdr:row>1</xdr:row>
-      <xdr:rowOff>52387</xdr:rowOff>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>23812</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>23812</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>14</xdr:col>
-      <xdr:colOff>466725</xdr:colOff>
-      <xdr:row>15</xdr:row>
-      <xdr:rowOff>128587</xdr:rowOff>
+      <xdr:col>22</xdr:col>
+      <xdr:colOff>328612</xdr:colOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>100012</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="3" name="Chart 2">
+        <xdr:cNvPr id="6" name="Chart 5">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E081E6CD-0FDB-4CA1-888E-4FBD23EBA1E5}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{0D576E4D-3191-43ED-84FC-E8F2819744DC}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3203,23 +5907,23 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>15</xdr:col>
-      <xdr:colOff>495300</xdr:colOff>
-      <xdr:row>2</xdr:row>
-      <xdr:rowOff>100012</xdr:rowOff>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>104775</xdr:colOff>
+      <xdr:row>15</xdr:row>
+      <xdr:rowOff>4762</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>23</xdr:col>
-      <xdr:colOff>190500</xdr:colOff>
-      <xdr:row>16</xdr:row>
-      <xdr:rowOff>176212</xdr:rowOff>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>409575</xdr:colOff>
+      <xdr:row>29</xdr:row>
+      <xdr:rowOff>80962</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="4" name="Chart 3">
+        <xdr:cNvPr id="2" name="Chart 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{01CE47D2-EA14-4AF2-B23E-E3E1CDCB1766}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{9DF92210-633C-4FF8-9302-E5CC449CA855}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3537,15 +6241,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{238B50C7-D4C4-4AC3-AC98-A793DE8FDB5E}">
-  <dimension ref="A1:G13"/>
+  <dimension ref="A1:G27"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="W2" sqref="W2"/>
+      <selection activeCell="B16" sqref="B16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="5" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="9.42578125" bestFit="1" customWidth="1"/>
     <col min="2" max="3" width="9" bestFit="1" customWidth="1"/>
     <col min="4" max="5" width="10" bestFit="1" customWidth="1"/>
     <col min="6" max="7" width="11" bestFit="1" customWidth="1"/>
@@ -3556,23 +6260,18 @@
         <v>1048576</v>
       </c>
       <c r="C1">
-        <f>2*B1</f>
         <v>2097152</v>
       </c>
       <c r="D1">
-        <f t="shared" ref="D1:G1" si="0">2*C1</f>
         <v>4194304</v>
       </c>
       <c r="E1">
-        <f t="shared" si="0"/>
         <v>8388608</v>
       </c>
       <c r="F1">
-        <f t="shared" si="0"/>
         <v>16777216</v>
       </c>
       <c r="G1">
-        <f t="shared" si="0"/>
         <v>33554432</v>
       </c>
     </row>
@@ -3721,6 +6420,18 @@
       <c r="B8">
         <v>9.7921999999999995E-2</v>
       </c>
+      <c r="C8">
+        <v>0.19584399999999999</v>
+      </c>
+      <c r="D8">
+        <v>0.39168799999999998</v>
+      </c>
+      <c r="E8">
+        <v>0.78337599999999996</v>
+      </c>
+      <c r="F8">
+        <v>1.5667519999999999</v>
+      </c>
       <c r="G8">
         <v>4.6071679999999997</v>
       </c>
@@ -3732,6 +6443,18 @@
       <c r="B9">
         <v>5.2689E-2</v>
       </c>
+      <c r="C9">
+        <v>0.105378</v>
+      </c>
+      <c r="D9">
+        <v>0.210756</v>
+      </c>
+      <c r="E9">
+        <v>0.421512</v>
+      </c>
+      <c r="F9">
+        <v>0.843024</v>
+      </c>
       <c r="G9">
         <v>2.4073449999999998</v>
       </c>
@@ -3743,6 +6466,18 @@
       <c r="B10">
         <v>3.048E-2</v>
       </c>
+      <c r="C10">
+        <v>6.096E-2</v>
+      </c>
+      <c r="D10">
+        <v>0.12192</v>
+      </c>
+      <c r="E10">
+        <v>0.24384</v>
+      </c>
+      <c r="F10">
+        <v>0.48768</v>
+      </c>
       <c r="G10">
         <v>1.3045929999999999</v>
       </c>
@@ -3754,6 +6489,18 @@
       <c r="B11">
         <v>1.9050000000000001E-2</v>
       </c>
+      <c r="C11">
+        <v>3.8100000000000002E-2</v>
+      </c>
+      <c r="D11">
+        <v>7.6200000000000004E-2</v>
+      </c>
+      <c r="E11">
+        <v>0.15240000000000001</v>
+      </c>
+      <c r="F11">
+        <v>0.30480000000000002</v>
+      </c>
       <c r="G11">
         <v>0.75179600000000002</v>
       </c>
@@ -3765,6 +6512,18 @@
       <c r="B12">
         <v>1.3672E-2</v>
       </c>
+      <c r="C12">
+        <v>2.7344E-2</v>
+      </c>
+      <c r="D12">
+        <v>5.4688000000000001E-2</v>
+      </c>
+      <c r="E12">
+        <v>0.109376</v>
+      </c>
+      <c r="F12">
+        <v>0.218752</v>
+      </c>
       <c r="G12">
         <v>0.47471099999999999</v>
       </c>
@@ -3776,8 +6535,339 @@
       <c r="B13">
         <v>1.2108000000000001E-2</v>
       </c>
+      <c r="C13">
+        <v>2.4216000000000001E-2</v>
+      </c>
+      <c r="D13">
+        <v>4.8432000000000003E-2</v>
+      </c>
+      <c r="E13">
+        <v>9.6864000000000006E-2</v>
+      </c>
+      <c r="F13">
+        <v>0.19372800000000001</v>
+      </c>
       <c r="G13">
         <v>0.36280200000000001</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>0</v>
+      </c>
+      <c r="B14">
+        <v>1.6255010000000001</v>
+      </c>
+      <c r="C14">
+        <v>3.5216780000000001</v>
+      </c>
+      <c r="D14">
+        <v>6.9416599999999997</v>
+      </c>
+      <c r="E14">
+        <v>14.582269</v>
+      </c>
+      <c r="F14">
+        <v>29.707936</v>
+      </c>
+      <c r="G14">
+        <v>63.788241999999997</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B15">
+        <v>1048576</v>
+      </c>
+      <c r="C15">
+        <v>2097152</v>
+      </c>
+      <c r="D15">
+        <v>4194304</v>
+      </c>
+      <c r="E15">
+        <v>8388608</v>
+      </c>
+      <c r="F15">
+        <v>16777216</v>
+      </c>
+      <c r="G15">
+        <v>33554432</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A16">
+        <v>2</v>
+      </c>
+      <c r="B16">
+        <v>0.28779123200000001</v>
+      </c>
+      <c r="C16">
+        <v>0.28399987700000001</v>
+      </c>
+      <c r="D16">
+        <v>0.25604921000000003</v>
+      </c>
+      <c r="E16">
+        <v>0.24696225299999999</v>
+      </c>
+      <c r="F16">
+        <v>0.231810561</v>
+      </c>
+      <c r="G16">
+        <v>0.22991808799999999</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A17">
+        <v>4</v>
+      </c>
+      <c r="B17">
+        <v>0.57334873500000005</v>
+      </c>
+      <c r="C17">
+        <v>0.566330852</v>
+      </c>
+      <c r="D17">
+        <v>0.510730727</v>
+      </c>
+      <c r="E17">
+        <v>0.49271257000000002</v>
+      </c>
+      <c r="F17">
+        <v>0.46254644</v>
+      </c>
+      <c r="G17">
+        <v>0.45914060400000001</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A18">
+        <v>8</v>
+      </c>
+      <c r="B18">
+        <v>1.140004054</v>
+      </c>
+      <c r="C18">
+        <v>1.1260368510000001</v>
+      </c>
+      <c r="D18">
+        <v>1.017100492</v>
+      </c>
+      <c r="E18">
+        <v>0.98157556999999995</v>
+      </c>
+      <c r="F18">
+        <v>0.92169960699999998</v>
+      </c>
+      <c r="G18">
+        <v>0.91517404099999999</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A19">
+        <v>16</v>
+      </c>
+      <c r="B19">
+        <v>2.2604721470000002</v>
+      </c>
+      <c r="C19">
+        <v>2.2350778099999999</v>
+      </c>
+      <c r="D19">
+        <v>2.0187829879999999</v>
+      </c>
+      <c r="E19">
+        <v>1.951442471</v>
+      </c>
+      <c r="F19">
+        <v>1.8329591169999999</v>
+      </c>
+      <c r="G19">
+        <v>1.8208358339999999</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A20">
+        <v>32</v>
+      </c>
+      <c r="B20">
+        <v>4.4526100690000003</v>
+      </c>
+      <c r="C20">
+        <v>4.4115271390000004</v>
+      </c>
+      <c r="D20">
+        <v>3.9891044189999998</v>
+      </c>
+      <c r="E20">
+        <v>3.8567269049999999</v>
+      </c>
+      <c r="F20">
+        <v>3.6326345500000001</v>
+      </c>
+      <c r="G20">
+        <v>3.6106461470000002</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A21">
+        <v>64</v>
+      </c>
+      <c r="B21">
+        <v>8.6890338099999997</v>
+      </c>
+      <c r="C21">
+        <v>8.6427908799999997</v>
+      </c>
+      <c r="D21">
+        <v>7.8346626879999999</v>
+      </c>
+      <c r="E21">
+        <v>7.5870759860000003</v>
+      </c>
+      <c r="F21">
+        <v>7.1393279820000002</v>
+      </c>
+      <c r="G21">
+        <v>7.1171470729999999</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A22">
+        <v>128</v>
+      </c>
+      <c r="B22">
+        <v>16.599957109999998</v>
+      </c>
+      <c r="C22">
+        <v>17.982057149999999</v>
+      </c>
+      <c r="D22">
+        <v>17.722421929999999</v>
+      </c>
+      <c r="E22">
+        <v>18.614648649999999</v>
+      </c>
+      <c r="F22">
+        <v>18.961479539999999</v>
+      </c>
+      <c r="G22">
+        <v>13.84543433</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A23">
+        <v>256</v>
+      </c>
+      <c r="B23">
+        <v>30.850860709999999</v>
+      </c>
+      <c r="C23">
+        <v>33.419480350000001</v>
+      </c>
+      <c r="D23">
+        <v>32.936950789999997</v>
+      </c>
+      <c r="E23">
+        <v>34.59514557</v>
+      </c>
+      <c r="F23">
+        <v>35.239727459999997</v>
+      </c>
+      <c r="G23">
+        <v>26.497341259999999</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A24">
+        <v>512</v>
+      </c>
+      <c r="B24">
+        <v>53.3300853</v>
+      </c>
+      <c r="C24">
+        <v>57.770308399999998</v>
+      </c>
+      <c r="D24">
+        <v>56.936187660000002</v>
+      </c>
+      <c r="E24">
+        <v>59.802612369999999</v>
+      </c>
+      <c r="F24">
+        <v>60.91686352</v>
+      </c>
+      <c r="G24">
+        <v>48.895128210000003</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A25">
+        <v>1024</v>
+      </c>
+      <c r="B25">
+        <v>85.328136479999998</v>
+      </c>
+      <c r="C25">
+        <v>92.432493440000002</v>
+      </c>
+      <c r="D25">
+        <v>91.097900260000003</v>
+      </c>
+      <c r="E25">
+        <v>95.684179790000002</v>
+      </c>
+      <c r="F25">
+        <v>97.466981630000006</v>
+      </c>
+      <c r="G25">
+        <v>84.847807119999999</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A26">
+        <v>2048</v>
+      </c>
+      <c r="B26">
+        <v>118.8927004</v>
+      </c>
+      <c r="C26">
+        <v>128.79161790000001</v>
+      </c>
+      <c r="D26">
+        <v>126.93205089999999</v>
+      </c>
+      <c r="E26">
+        <v>133.32238330000001</v>
+      </c>
+      <c r="F26">
+        <v>135.80646580000001</v>
+      </c>
+      <c r="G26">
+        <v>134.37279100000001</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A27">
+        <v>4096</v>
+      </c>
+      <c r="B27">
+        <v>134.2501652</v>
+      </c>
+      <c r="C27">
+        <v>145.4277337</v>
+      </c>
+      <c r="D27">
+        <v>143.32796500000001</v>
+      </c>
+      <c r="E27">
+        <v>150.5437417</v>
+      </c>
+      <c r="F27">
+        <v>153.34869509999999</v>
+      </c>
+      <c r="G27">
+        <v>175.82108700000001</v>
       </c>
     </row>
   </sheetData>

</xml_diff>